<commit_message>
SO,Argentine basin, Irminger HYPM cal and ingest sheet changes
added engineerign idata streams for 2nfd WFP where necessary
Corrected FLORD L cal parameters
Set CTDMO Modem ID
</commit_message>
<xml_diff>
--- a/GA02HYPM/Omaha_Cal_Info_GA02HYPM_00001.xlsx
+++ b/GA02HYPM/Omaha_Cal_Info_GA02HYPM_00001.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Documents\Project Info\WHOI\Marine Integration - OOI\OOInet Migration\Integration\Cal and Ingest Sheets\Sheets from -test 2015-08-19\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9612"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20160" windowHeight="9555" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -22,12 +17,12 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="52">
   <si>
     <t>Ref Des</t>
   </si>
@@ -173,19 +168,16 @@
     <t>GA03HYPM-GP-00001-ENG</t>
   </si>
   <si>
-    <t>GA03HYPM-WFP-00001-ENG</t>
-  </si>
-  <si>
     <t>GA02HYPM-GP001-00-ENG000000</t>
   </si>
   <si>
-    <t>GA02HYPM-RIS01-46-CTDMOG000</t>
-  </si>
-  <si>
-    <t>This reference designator is incorrect - should be GA02HYPM-RIS01-01-CTDMOG039 but it was set by the parser to follow the imductive modem ID</t>
-  </si>
-  <si>
     <t>GA02HYPM</t>
+  </si>
+  <si>
+    <t>GA02HYPM-RIM01-02-CTDMOG046</t>
+  </si>
+  <si>
+    <t>GA02HYPM-WFP03-00-ENG000000</t>
   </si>
 </sst>
 </file>
@@ -198,7 +190,7 @@
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,8 +347,129 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,8 +505,176 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -455,8 +736,115 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="131">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -588,8 +976,50 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -655,9 +1085,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -667,8 +1094,41 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="131">
+  <cellStyles count="173">
+    <cellStyle name="20% - Accent1" xfId="149" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="153" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="157" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="161" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="165" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="169" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="150" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="154" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="158" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="162" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="166" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="170" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="151" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="155" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="159" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="163" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="167" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="171" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="148" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="152" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="156" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="160" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="164" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="168" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="137" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="141" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="143" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Comma 2" xfId="62"/>
     <cellStyle name="Comma 2 2" xfId="63"/>
     <cellStyle name="Comma 2 2 2" xfId="64"/>
@@ -679,6 +1139,12 @@
     <cellStyle name="Currency 2 3" xfId="69"/>
     <cellStyle name="Excel Built-in Normal" xfId="5"/>
     <cellStyle name="Excel Built-in Normal 2" xfId="70"/>
+    <cellStyle name="Explanatory Text" xfId="146" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="136" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="132" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="133" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="134" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="135" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink 2" xfId="8"/>
     <cellStyle name="Hyperlink 2 2" xfId="71"/>
     <cellStyle name="Hyperlink 2 3" xfId="72"/>
@@ -693,10 +1159,14 @@
     <cellStyle name="Hyperlink 7" xfId="13"/>
     <cellStyle name="Hyperlink 7 2" xfId="77"/>
     <cellStyle name="Hyperlink 8" xfId="14"/>
+    <cellStyle name="Input" xfId="139" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="142" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="138" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Neutral 2" xfId="78"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="15"/>
     <cellStyle name="Normal 11" xfId="16"/>
+    <cellStyle name="Normal 11 2" xfId="172"/>
     <cellStyle name="Normal 12" xfId="17"/>
     <cellStyle name="Normal 13" xfId="18"/>
     <cellStyle name="Normal 14" xfId="57"/>
@@ -780,8 +1250,12 @@
     <cellStyle name="Normal 7" xfId="45"/>
     <cellStyle name="Normal 8" xfId="46"/>
     <cellStyle name="Normal 9" xfId="47"/>
+    <cellStyle name="Note" xfId="145" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="140" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Percent 2" xfId="121"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
+    <cellStyle name="Title" xfId="131" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="147" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Untitled1" xfId="48"/>
     <cellStyle name="Untitled1 2" xfId="122"/>
     <cellStyle name="Untitled2" xfId="49"/>
@@ -800,15 +1274,13 @@
     <cellStyle name="Untitled8 2" xfId="129"/>
     <cellStyle name="Untitled9" xfId="56"/>
     <cellStyle name="Untitled9 2" xfId="130"/>
+    <cellStyle name="Warning Text" xfId="144" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -874,7 +1346,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -909,7 +1381,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1120,26 +1592,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="17.109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.88671875" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="7" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -1177,9 +1649,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
-        <v>52</v>
+    <row r="2" spans="1:13" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>49</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>30</v>
@@ -1216,48 +1688,48 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
       <c r="D3" s="19"/>
       <c r="E3" s="20"/>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
       <c r="D10" s="19"/>
       <c r="E10" s="20"/>
       <c r="F10" s="19"/>
     </row>
-    <row r="11" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
       <c r="F11" s="19"/>
     </row>
-    <row r="12" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
       <c r="F12" s="19"/>
     </row>
-    <row r="13" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
       <c r="F13" s="19"/>
     </row>
-    <row r="14" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
       <c r="D14" s="19"/>
       <c r="E14" s="20"/>
       <c r="F14" s="19"/>
     </row>
-    <row r="15" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
       <c r="F15" s="19"/>
     </row>
-    <row r="16" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
       <c r="D16" s="19"/>
       <c r="E16" s="20"/>
       <c r="F16" s="19"/>
@@ -1270,25 +1742,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="78.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="26.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="78.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="10" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1311,8 +1783,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="10" customFormat="1" ht="13.9" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1335,7 +1807,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1355,7 +1827,7 @@
         <v>1.7379999999999999E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1375,7 +1847,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1395,7 +1867,7 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1412,13 +1884,13 @@
         <v>26</v>
       </c>
       <c r="F7" s="1">
-        <v>117</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="G7" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1441,7 +1913,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1458,13 +1930,13 @@
         <v>28</v>
       </c>
       <c r="F9" s="1">
-        <v>1.08</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1487,7 +1959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1510,7 +1982,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1530,7 +2002,7 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -1550,7 +2022,7 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1570,7 +2042,7 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1590,7 +2062,7 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -1610,7 +2082,7 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1633,7 +2105,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -1653,7 +2125,7 @@
         <v>1.702E-6</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -1673,7 +2145,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -1693,7 +2165,7 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
@@ -1710,13 +2182,13 @@
         <v>26</v>
       </c>
       <c r="F25" s="1">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1739,7 +2211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
@@ -1756,13 +2228,13 @@
         <v>28</v>
       </c>
       <c r="F27" s="1">
-        <v>1.08</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
@@ -1785,7 +2257,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -1805,7 +2277,7 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
@@ -1825,7 +2297,7 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -1845,7 +2317,7 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
@@ -1865,7 +2337,7 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -1885,7 +2357,7 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -1905,13 +2377,13 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G39" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="25" t="s">
+    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="27" t="s">
         <v>50</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1927,14 +2399,12 @@
         <v>5</v>
       </c>
       <c r="F41" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G41" s="25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="25" t="s">
+        <v>1470</v>
+      </c>
+      <c r="G41" s="24"/>
+    </row>
+    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="28" t="s">
         <v>50</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1952,12 +2422,10 @@
       <c r="F42" s="1">
         <v>-42.981666666666669</v>
       </c>
-      <c r="G42" s="25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="25" t="s">
+      <c r="G42" s="24"/>
+    </row>
+    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="29" t="s">
         <v>50</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1975,13 +2443,11 @@
       <c r="F43" s="1">
         <v>-42.4985</v>
       </c>
-      <c r="G43" s="25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G43" s="24"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>30</v>
@@ -1989,16 +2455,16 @@
       <c r="C45" s="1">
         <v>1</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="25" t="s">
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
         <v>45</v>
       </c>
@@ -2008,12 +2474,25 @@
       <c r="C46" s="1">
         <v>1</v>
       </c>
-      <c r="D46" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="G46" s="25" t="s">
-        <v>46</v>
-      </c>
+      <c r="D46" s="26">
+        <v>1399421</v>
+      </c>
+      <c r="G46" s="24"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47" s="26">
+        <v>1399422</v>
+      </c>
+      <c r="G47" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor corrections to HYPM cal and ingest sheets
Corrected a couple reference designators.  Made the reference designator
in the ingest sheet for the CTDMO match the reference designator list.
Made the CTDMO reference designator in the cal sheet include the IMM.
</commit_message>
<xml_diff>
--- a/GA02HYPM/Omaha_Cal_Info_GA02HYPM_00001.xlsx
+++ b/GA02HYPM/Omaha_Cal_Info_GA02HYPM_00001.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="51">
   <si>
     <t>Ref Des</t>
   </si>
@@ -162,9 +162,6 @@
     <t>GA02HYPM-WFP02-00-ENG000000</t>
   </si>
   <si>
-    <t>The serial number used here is bogus, pending identification of the real serial number.</t>
-  </si>
-  <si>
     <t>GA03HYPM-GP-00001-ENG</t>
   </si>
   <si>
@@ -174,10 +171,10 @@
     <t>GA02HYPM</t>
   </si>
   <si>
+    <t>GA02HYPM-WFP03-00-ENG000000</t>
+  </si>
+  <si>
     <t>GA02HYPM-RIM01-02-CTDMOG046</t>
-  </si>
-  <si>
-    <t>GA02HYPM-WFP03-00-ENG000000</t>
   </si>
 </sst>
 </file>
@@ -1651,7 +1648,7 @@
     </row>
     <row r="2" spans="1:13" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>30</v>
@@ -1744,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2447,7 +2444,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>30</v>
@@ -2456,13 +2453,11 @@
         <v>1</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E45" s="23"/>
       <c r="F45" s="23"/>
-      <c r="G45" s="24" t="s">
-        <v>46</v>
-      </c>
+      <c r="G45" s="24"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
@@ -2481,7 +2476,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
redmine #9271 cal sheets for GA01SUMO, GA02HYPM, GA03FLMA, GA03FLMB, GA05MOAS gliders 493,393 and 496 modified in repo.
</commit_message>
<xml_diff>
--- a/GA02HYPM/Omaha_Cal_Info_GA02HYPM_00001.xlsx
+++ b/GA02HYPM/Omaha_Cal_Info_GA02HYPM_00001.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20160" windowHeight="9555" activeTab="1"/>
+    <workbookView xWindow="5440" yWindow="7720" windowWidth="26840" windowHeight="10160"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -17,12 +17,17 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="53">
   <si>
     <t>Ref Des</t>
   </si>
@@ -153,18 +158,12 @@
     <t>42° 29.91' W</t>
   </si>
   <si>
-    <t>AT26-30</t>
-  </si>
-  <si>
     <t>GA02HYPM-MFC04-01-ZPLSGA000 unit not deployed</t>
   </si>
   <si>
     <t>GA02HYPM-WFP02-00-ENG000000</t>
   </si>
   <si>
-    <t>GA03HYPM-GP-00001-ENG</t>
-  </si>
-  <si>
     <t>GA02HYPM-GP001-00-ENG000000</t>
   </si>
   <si>
@@ -175,6 +174,56 @@
   </si>
   <si>
     <t>GA02HYPM-RIM01-02-CTDMOG046</t>
+  </si>
+  <si>
+    <r>
+      <t>AT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>26-30</t>
+    </r>
+  </si>
+  <si>
+    <t>13104-04</t>
+  </si>
+  <si>
+    <t>13104-06</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>37-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12406</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -182,12 +231,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,6 +513,33 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="37">
@@ -707,16 +783,16 @@
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -841,7 +917,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="173">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -904,14 +980,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1015,8 +1091,34 @@
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="40" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1039,19 +1141,19 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1075,10 +1177,10 @@
     <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1091,14 +1193,20 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="173">
+  <cellStyles count="199">
     <cellStyle name="20% - Accent1" xfId="149" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="153" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="157" builtinId="38" customBuiltin="1"/>
@@ -1137,11 +1245,37 @@
     <cellStyle name="Excel Built-in Normal" xfId="5"/>
     <cellStyle name="Excel Built-in Normal 2" xfId="70"/>
     <cellStyle name="Explanatory Text" xfId="146" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="136" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="132" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="133" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="134" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="135" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="8"/>
     <cellStyle name="Hyperlink 2 2" xfId="71"/>
     <cellStyle name="Hyperlink 2 3" xfId="72"/>
@@ -1284,7 +1418,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1589,29 +1723,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="28">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1646,9 +1780,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="13" customFormat="1">
       <c r="A2" s="25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>30</v>
@@ -1673,7 +1807,7 @@
         <v>5200</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="18">
@@ -1685,55 +1819,60 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="13" customFormat="1">
       <c r="D3" s="19"/>
       <c r="E3" s="20"/>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" customFormat="1"/>
+    <row r="5" spans="1:13" customFormat="1"/>
+    <row r="6" spans="1:13" customFormat="1"/>
+    <row r="7" spans="1:13" customFormat="1"/>
+    <row r="8" spans="1:13" customFormat="1"/>
+    <row r="9" spans="1:13" customFormat="1"/>
+    <row r="10" spans="1:13" s="13" customFormat="1">
       <c r="D10" s="19"/>
       <c r="E10" s="20"/>
       <c r="F10" s="19"/>
     </row>
-    <row r="11" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="13" customFormat="1">
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
       <c r="F11" s="19"/>
     </row>
-    <row r="12" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="13" customFormat="1">
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
       <c r="F12" s="19"/>
     </row>
-    <row r="13" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" s="13" customFormat="1">
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
       <c r="F13" s="19"/>
     </row>
-    <row r="14" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" s="13" customFormat="1">
       <c r="D14" s="19"/>
       <c r="E14" s="20"/>
       <c r="F14" s="19"/>
     </row>
-    <row r="15" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" s="13" customFormat="1">
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
       <c r="F15" s="19"/>
     </row>
-    <row r="16" spans="1:13" s="13" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" s="13" customFormat="1">
       <c r="D16" s="19"/>
       <c r="E16" s="20"/>
       <c r="F16" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1741,23 +1880,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="78.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="26.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="78.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="10" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="10" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1780,8 +1919,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="10" customFormat="1" ht="13.9" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="10" customFormat="1"/>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1804,7 +1943,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1824,7 +1963,7 @@
         <v>1.7379999999999999E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1844,7 +1983,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1864,7 +2003,7 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1887,7 +2026,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1910,7 +2049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1926,14 +2065,14 @@
       <c r="E9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="1">
-        <v>1.1299999999999999</v>
+      <c r="F9" s="31">
+        <v>1.0960000000000001</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1956,7 +2095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1979,7 +2118,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1999,7 +2138,7 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -2019,7 +2158,7 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -2039,7 +2178,7 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -2059,7 +2198,7 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -2079,7 +2218,7 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -2102,7 +2241,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -2122,7 +2261,7 @@
         <v>1.702E-6</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -2142,7 +2281,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -2162,7 +2301,7 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
@@ -2185,7 +2324,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -2208,7 +2347,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
@@ -2231,7 +2370,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
@@ -2254,7 +2393,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -2274,7 +2413,7 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
@@ -2294,7 +2433,7 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -2314,7 +2453,7 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
@@ -2334,7 +2473,7 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -2354,7 +2493,7 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -2374,14 +2513,14 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="G39" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="27" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="26" t="s">
+        <v>48</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>30</v>
@@ -2389,20 +2528,20 @@
       <c r="C41" s="1">
         <v>1</v>
       </c>
-      <c r="D41" s="1">
-        <v>12406</v>
+      <c r="D41" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="1">
-        <v>1470</v>
+      <c r="F41" s="30">
+        <v>1450</v>
       </c>
       <c r="G41" s="24"/>
     </row>
-    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
-        <v>50</v>
+    <row r="42" spans="1:7">
+      <c r="A42" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>30</v>
@@ -2410,8 +2549,8 @@
       <c r="C42" s="1">
         <v>1</v>
       </c>
-      <c r="D42" s="1">
-        <v>12406</v>
+      <c r="D42" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>6</v>
@@ -2421,9 +2560,9 @@
       </c>
       <c r="G42" s="24"/>
     </row>
-    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="29" t="s">
-        <v>50</v>
+    <row r="43" spans="1:7">
+      <c r="A43" s="28" t="s">
+        <v>48</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>30</v>
@@ -2431,8 +2570,8 @@
       <c r="C43" s="1">
         <v>1</v>
       </c>
-      <c r="D43" s="1">
-        <v>12406</v>
+      <c r="D43" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>7</v>
@@ -2442,9 +2581,9 @@
       </c>
       <c r="G43" s="24"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" s="22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>30</v>
@@ -2452,16 +2591,16 @@
       <c r="C45" s="1">
         <v>1</v>
       </c>
-      <c r="D45" s="26" t="s">
-        <v>46</v>
+      <c r="D45" s="29">
+        <v>13994</v>
       </c>
       <c r="E45" s="23"/>
       <c r="F45" s="23"/>
       <c r="G45" s="24"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>30</v>
@@ -2469,14 +2608,14 @@
       <c r="C46" s="1">
         <v>1</v>
       </c>
-      <c r="D46" s="26">
-        <v>1399421</v>
+      <c r="D46" s="29" t="s">
+        <v>50</v>
       </c>
       <c r="G46" s="24"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>30</v>
@@ -2484,13 +2623,18 @@
       <c r="C47" s="1">
         <v>1</v>
       </c>
-      <c r="D47" s="26">
-        <v>1399422</v>
+      <c r="D47" s="29" t="s">
+        <v>51</v>
       </c>
       <c r="G47" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>